<commit_message>
se hacen archivos diferentes para nuevas restricciones
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -101,13 +101,13 @@
     <t>INGLÉS</t>
   </si>
   <si>
-    <t>CIENCIAS NATURALES</t>
-  </si>
-  <si>
     <t>MATEMÁTICA</t>
   </si>
   <si>
     <t>LENGUAJE</t>
+  </si>
+  <si>
+    <t>CIENCIAS NATURALES</t>
   </si>
   <si>
     <t>HISTORIA</t>
@@ -140,16 +140,19 @@
     <t>3A</t>
   </si>
   <si>
-    <t>5B</t>
+    <t>7A</t>
   </si>
   <si>
-    <t>7A</t>
+    <t>5B</t>
   </si>
   <si>
     <t>2B</t>
   </si>
   <si>
     <t>2A</t>
+  </si>
+  <si>
+    <t>8A</t>
   </si>
   <si>
     <t>8B</t>
@@ -159,9 +162,6 @@
   </si>
   <si>
     <t>4B</t>
-  </si>
-  <si>
-    <t>8A</t>
   </si>
 </sst>
 </file>
@@ -743,9 +743,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s"/>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
+      <c r="D3" t="s"/>
       <c r="E3" t="s">
         <v>5</v>
       </c>
@@ -759,7 +757,7 @@
       </c>
       <c r="B4" t="s"/>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -773,11 +771,9 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
+      <c r="B5" t="s"/>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -794,7 +790,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -813,17 +809,19 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
+      <c r="B7" t="s"/>
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s"/>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
-      <c r="F7" t="s"/>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="n">
@@ -851,7 +849,9 @@
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s"/>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
       <c r="E9" t="s">
         <v>5</v>
       </c>
@@ -926,7 +926,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -959,9 +959,7 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
+      <c r="D5" t="s"/>
       <c r="E5" t="s">
         <v>5</v>
       </c>
@@ -1025,7 +1023,9 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="s"/>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
@@ -1083,13 +1083,17 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s"/>
-      <c r="F2" t="s"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="n">
@@ -1118,9 +1122,7 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
+      <c r="C4" t="s"/>
       <c r="D4" t="s">
         <v>5</v>
       </c>
@@ -1151,7 +1153,9 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="s"/>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
@@ -1197,9 +1201,7 @@
       <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="F8" t="s">
-        <v>5</v>
-      </c>
+      <c r="F8" t="s"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="n">
@@ -1215,9 +1217,7 @@
         <v>5</v>
       </c>
       <c r="E9" t="s"/>
-      <c r="F9" t="s">
-        <v>6</v>
-      </c>
+      <c r="F9" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -1260,19 +1260,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
       </c>
       <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1284,12 +1284,14 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s"/>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="n">
@@ -1299,7 +1301,7 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -1316,31 +1318,31 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s"/>
+      <c r="B6" t="s"/>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
@@ -1353,16 +1355,16 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="s"/>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
       <c r="C7" t="s"/>
-      <c r="D7" t="s">
+      <c r="D7" t="s"/>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
         <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1370,16 +1372,14 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s"/>
+      <c r="E8" t="s">
         <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
@@ -1390,17 +1390,17 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s"/>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1444,10 +1444,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -1464,32 +1464,32 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s"/>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s"/>
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
+      <c r="B4" t="s"/>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
@@ -1499,7 +1499,9 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="s"/>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
@@ -1510,7 +1512,7 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1518,19 +1520,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1541,16 +1543,16 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1558,10 +1560,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
       </c>
       <c r="D8" t="s"/>
       <c r="E8" t="s"/>
@@ -1575,17 +1577,15 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
+      <c r="F9" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -1631,13 +1631,13 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -1660,7 +1660,7 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1668,10 +1668,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -1686,38 +1686,36 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F5" t="s"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s"/>
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
       <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F6" t="s"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="n">
@@ -1727,16 +1725,16 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1746,9 +1744,11 @@
       <c r="B8" t="s"/>
       <c r="C8" t="s"/>
       <c r="D8" t="s"/>
-      <c r="E8" t="s"/>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1762,13 +1762,13 @@
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1812,16 +1812,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1834,12 +1834,8 @@
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
+      <c r="C3" t="s"/>
+      <c r="D3" t="s"/>
       <c r="E3" t="s">
         <v>16</v>
       </c>
@@ -1852,17 +1848,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s"/>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1870,17 +1866,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s"/>
       <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1888,19 +1886,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1908,7 +1906,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -1927,7 +1925,7 @@
       </c>
       <c r="B8" t="s"/>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s"/>
       <c r="E8" t="s">
@@ -1942,18 +1940,20 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
         <v>13</v>
       </c>
-      <c r="F9" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -2041,7 +2041,9 @@
       </c>
       <c r="D5" t="s"/>
       <c r="E5" t="s"/>
-      <c r="F5" t="s"/>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="n">
@@ -2061,7 +2063,9 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="s"/>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" t="s"/>
       <c r="D7" t="s"/>
       <c r="E7" t="s"/>
@@ -2208,18 +2212,18 @@
       </c>
       <c r="C5" t="s"/>
       <c r="D5" t="s"/>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
+      <c r="E5" t="s"/>
       <c r="F5" t="s"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="s"/>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s"/>
       <c r="E6" t="s"/>
@@ -2229,7 +2233,9 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="s"/>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
       <c r="C7" t="s"/>
       <c r="D7" t="s"/>
       <c r="E7" t="s"/>
@@ -2253,7 +2259,9 @@
       <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s"/>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
       <c r="E9" t="s"/>
       <c r="F9" t="s"/>
     </row>
@@ -2335,7 +2343,9 @@
       </c>
       <c r="D2" t="s"/>
       <c r="E2" t="s"/>
-      <c r="F2" t="s"/>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="n">
@@ -2345,12 +2355,10 @@
         <v>17</v>
       </c>
       <c r="C3" t="s"/>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
+      <c r="D3" t="s"/>
       <c r="E3" t="s"/>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2361,9 +2369,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s"/>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
+      <c r="D4" t="s"/>
       <c r="E4" t="s"/>
       <c r="F4" t="s"/>
     </row>
@@ -2390,7 +2396,7 @@
       <c r="D6" t="s"/>
       <c r="E6" t="s"/>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2404,20 +2410,18 @@
       <c r="D7" t="s"/>
       <c r="E7" t="s"/>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
+      <c r="B8" t="s"/>
       <c r="C8" t="s"/>
       <c r="D8" t="s"/>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s"/>
     </row>
@@ -2507,21 +2511,19 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s"/>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
+      <c r="B3" t="s"/>
       <c r="C3" t="s">
         <v>5</v>
       </c>
@@ -2544,7 +2546,9 @@
         <v>5</v>
       </c>
       <c r="D4" t="s"/>
-      <c r="E4" t="s"/>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
       <c r="F4" t="s">
         <v>5</v>
       </c>
@@ -2576,9 +2580,7 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
+      <c r="C6" t="s"/>
       <c r="D6" t="s">
         <v>5</v>
       </c>
@@ -2613,9 +2615,11 @@
       </c>
       <c r="B8" t="s"/>
       <c r="C8" t="s"/>
-      <c r="D8" t="s"/>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -2635,7 +2639,7 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
         <v>5</v>
@@ -2722,7 +2726,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -2731,7 +2735,7 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s"/>
     </row>
@@ -2752,7 +2756,7 @@
         <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2808,9 +2812,7 @@
       <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
+      <c r="E8" t="s"/>
       <c r="F8" t="s"/>
     </row>
     <row r="9" spans="1:6">
@@ -2821,14 +2823,12 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
+      <c r="E9" t="s"/>
       <c r="F9" t="s"/>
     </row>
     <row r="10" spans="1:6">
@@ -2908,10 +2908,10 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -2922,7 +2922,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -2934,7 +2934,7 @@
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2942,13 +2942,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
@@ -2965,16 +2965,16 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2982,7 +2982,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -2994,7 +2994,7 @@
         <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3025,7 +3025,7 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
@@ -3048,7 +3048,7 @@
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -3067,9 +3067,7 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
+      <c r="D10" t="s"/>
       <c r="E10" t="s"/>
       <c r="F10" t="s"/>
     </row>
@@ -3094,9 +3092,7 @@
       <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
+      <c r="C12" t="s"/>
       <c r="D12" t="s"/>
       <c r="E12" t="s"/>
       <c r="F12" t="s"/>
@@ -3173,9 +3169,7 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
+      <c r="F3" t="s"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="n">
@@ -3188,7 +3182,7 @@
         <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
@@ -3223,7 +3217,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
@@ -3241,7 +3235,7 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -3249,14 +3243,16 @@
       <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" t="s"/>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
@@ -3267,9 +3263,7 @@
       <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
+      <c r="F8" t="s"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="n">
@@ -3284,9 +3278,7 @@
       <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
+      <c r="E9" t="s"/>
       <c r="F9" t="s">
         <v>22</v>
       </c>
@@ -3367,9 +3359,7 @@
       <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
+      <c r="D2" t="s"/>
       <c r="E2" t="s"/>
       <c r="F2" t="s"/>
     </row>
@@ -3378,14 +3368,12 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
+      <c r="D3" t="s"/>
       <c r="E3" t="s">
         <v>29</v>
       </c>
@@ -3405,7 +3393,7 @@
       </c>
       <c r="D4" t="s"/>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s"/>
     </row>
@@ -3436,12 +3424,10 @@
         <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s"/>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
+      <c r="F6" t="s"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="n">
@@ -3482,7 +3468,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
@@ -3570,9 +3556,7 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
+      <c r="E2" t="s"/>
       <c r="F2" t="s"/>
     </row>
     <row r="3" spans="1:6">
@@ -3583,14 +3567,12 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
+      <c r="E3" t="s"/>
       <c r="F3" t="s"/>
     </row>
     <row r="4" spans="1:6">
@@ -3618,7 +3600,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -3659,7 +3641,7 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -3779,10 +3761,10 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
@@ -3796,7 +3778,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -3807,17 +3789,19 @@
       <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s"/>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
@@ -3854,7 +3838,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -3865,7 +3849,9 @@
       <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s"/>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="n">
@@ -3880,7 +3866,9 @@
       <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="E7" t="s"/>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
       <c r="F7" t="s"/>
     </row>
     <row r="8" spans="1:6">
@@ -3896,7 +3884,9 @@
       <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" t="s"/>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
       <c r="F8" t="s">
         <v>18</v>
       </c>
@@ -3912,7 +3902,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
         <v>28</v>
@@ -4035,7 +4025,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -4075,7 +4065,7 @@
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -4083,7 +4073,9 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s"/>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="n">
@@ -4101,7 +4093,9 @@
       <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="F7" t="s"/>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="n">
@@ -4128,7 +4122,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
@@ -4139,13 +4133,17 @@
       <c r="E9" t="s">
         <v>23</v>
       </c>
-      <c r="F9" t="s"/>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="s"/>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
       <c r="C10" t="s"/>
       <c r="D10" t="s"/>
       <c r="E10" t="s"/>
@@ -4155,7 +4153,9 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="s"/>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
       <c r="C11" t="s"/>
       <c r="D11" t="s"/>
       <c r="E11" t="s"/>
@@ -4212,7 +4212,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -4221,7 +4221,7 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
         <v>22</v>
@@ -4238,7 +4238,7 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
@@ -4333,7 +4333,7 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -4436,7 +4436,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -4452,19 +4452,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
       </c>
       <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -4472,7 +4472,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -4481,7 +4481,7 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
@@ -4492,10 +4492,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s"/>
       <c r="E5" t="s"/>
@@ -4527,7 +4527,7 @@
       </c>
       <c r="D7" t="s"/>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s"/>
     </row>
@@ -4542,11 +4542,11 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s"/>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -4636,19 +4636,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -4656,7 +4656,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -4667,28 +4667,26 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
+      <c r="F3" t="s"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -4696,7 +4694,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -4705,10 +4703,10 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -4716,10 +4714,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -4728,7 +4726,7 @@
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4747,19 +4745,17 @@
       <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
+      <c r="F7" t="s"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
@@ -4768,7 +4764,7 @@
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -4776,16 +4772,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="F9" t="s"/>
     </row>
@@ -4889,7 +4885,7 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -4902,7 +4898,9 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s"/>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
@@ -4944,13 +4942,13 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4961,9 +4959,7 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
+      <c r="D7" t="s"/>
       <c r="E7" t="s"/>
       <c r="F7" t="s">
         <v>5</v>
@@ -4974,7 +4970,9 @@
         <v>6</v>
       </c>
       <c r="B8" t="s"/>
-      <c r="C8" t="s"/>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
@@ -4993,9 +4991,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s"/>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D9" t="s"/>
       <c r="E9" t="s"/>
       <c r="F9" t="s"/>
     </row>
@@ -5040,10 +5036,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
@@ -5060,7 +5056,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -5069,7 +5065,7 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -5092,7 +5088,7 @@
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -5100,7 +5096,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -5112,7 +5108,7 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5120,7 +5116,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -5132,7 +5128,7 @@
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5146,7 +5142,7 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
@@ -5163,7 +5159,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
@@ -5183,7 +5179,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -5192,7 +5188,7 @@
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5266,19 +5262,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
-      </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -5286,15 +5282,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s"/>
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
       <c r="F3" t="s"/>
     </row>
     <row r="4" spans="1:6">
@@ -5305,12 +5303,14 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s"/>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
       <c r="F4" t="s"/>
     </row>
     <row r="5" spans="1:6">
@@ -5321,7 +5321,7 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -5339,30 +5339,32 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" t="s"/>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s"/>
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
       <c r="F7" t="s"/>
     </row>
     <row r="8" spans="1:6">
@@ -5373,11 +5375,13 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s"/>
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
         <v>21</v>
@@ -5388,18 +5392,18 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s"/>
+      <c r="F9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" t="s"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="n">
@@ -5481,22 +5485,24 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s"/>
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
@@ -5513,7 +5519,7 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -5521,50 +5527,56 @@
       <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s"/>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" t="s"/>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s"/>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -5573,7 +5585,7 @@
         <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -5608,13 +5620,13 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5691,7 +5703,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -5713,7 +5725,7 @@
       </c>
       <c r="D3" t="s"/>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s"/>
     </row>
@@ -5725,7 +5737,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s"/>
       <c r="E4" t="s"/>
@@ -5742,11 +5754,11 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s"/>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5759,9 +5771,11 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s"/>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
         <v>21</v>
@@ -5778,7 +5792,7 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
@@ -5790,7 +5804,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -5798,7 +5812,7 @@
       <c r="D8" t="s"/>
       <c r="E8" t="s"/>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -5806,15 +5820,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C9" t="s"/>
       <c r="D9" t="s"/>
       <c r="E9" t="s"/>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5891,7 +5903,7 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -5908,10 +5920,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -5920,7 +5932,7 @@
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -5937,10 +5949,10 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -5954,13 +5966,13 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5974,13 +5986,13 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
         <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5991,7 +6003,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -6014,7 +6026,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
@@ -6031,16 +6043,16 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -6114,19 +6126,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
       </c>
       <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -6134,19 +6146,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6154,19 +6166,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -6174,16 +6186,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
         <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -6194,7 +6206,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -6203,10 +6215,10 @@
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6217,7 +6229,7 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -6234,7 +6246,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -6243,7 +6255,7 @@
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
         <v>19</v>
@@ -6254,16 +6266,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
         <v>21</v>
@@ -6377,10 +6389,10 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -6391,10 +6403,10 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s"/>
       <c r="F3" t="s"/>
@@ -6413,7 +6425,7 @@
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s"/>
     </row>
@@ -6422,38 +6434,32 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
+      <c r="D5" t="s"/>
       <c r="E5" t="s"/>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
+      <c r="F5" t="s"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F6" t="s"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="n">
@@ -6465,9 +6471,7 @@
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
+      <c r="D7" t="s"/>
       <c r="E7" t="s"/>
       <c r="F7" t="s">
         <v>20</v>
@@ -6484,9 +6488,11 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s"/>
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
       <c r="F8" t="s"/>
     </row>
     <row r="9" spans="1:6">
@@ -6500,11 +6506,11 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s"/>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -6581,7 +6587,7 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -6644,21 +6650,17 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E5" t="s"/>
+      <c r="F5" t="s"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -6667,10 +6669,10 @@
         <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6684,7 +6686,7 @@
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s"/>
       <c r="F7" t="s">
@@ -6704,9 +6706,7 @@
       <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
+      <c r="E8" t="s"/>
       <c r="F8" t="s"/>
     </row>
     <row r="9" spans="1:6">
@@ -6722,7 +6722,9 @@
       <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" t="s"/>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
       <c r="F9" t="s">
         <v>24</v>
       </c>
@@ -6820,7 +6822,7 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -6843,10 +6845,10 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
         <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -6854,10 +6856,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -6872,15 +6874,17 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s"/>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
       <c r="E6" t="s"/>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6891,7 +6895,7 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s"/>
       <c r="E7" t="s"/>
@@ -6911,7 +6915,7 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
         <v>29</v>
@@ -6928,14 +6932,12 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="F9" t="s">
-        <v>19</v>
-      </c>
+      <c r="F9" t="s"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="n">
@@ -7011,7 +7013,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
@@ -7020,7 +7022,7 @@
         <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -7028,7 +7030,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -7037,7 +7039,7 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
@@ -7048,16 +7050,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
         <v>21</v>
@@ -7071,7 +7073,7 @@
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
         <v>28</v>
@@ -7088,19 +7090,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -7108,16 +7110,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -7131,16 +7133,16 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -7151,7 +7153,7 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -7160,7 +7162,7 @@
         <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -7273,15 +7275,15 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
+      <c r="F2" t="s"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="s"/>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -7299,7 +7301,9 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="s"/>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
@@ -7337,14 +7341,12 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
+      <c r="D6" t="s"/>
       <c r="E6" t="s">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -7354,9 +7356,7 @@
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
+      <c r="C7" t="s"/>
       <c r="D7" t="s">
         <v>5</v>
       </c>
@@ -7376,7 +7376,9 @@
       <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" t="s"/>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
       <c r="F8" t="s">
         <v>5</v>
       </c>
@@ -7442,19 +7444,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
       </c>
       <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
         <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -7465,13 +7467,13 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
         <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
       </c>
       <c r="F3" t="s">
         <v>21</v>
@@ -7482,19 +7484,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
         <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -7514,7 +7516,7 @@
         <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -7534,7 +7536,7 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -7542,19 +7544,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
         <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -7571,7 +7573,7 @@
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
@@ -7585,13 +7587,13 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
         <v>23</v>
@@ -7734,11 +7736,11 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s"/>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s"/>
       <c r="F5" t="s"/>
@@ -7753,7 +7755,7 @@
       <c r="C6" t="s"/>
       <c r="D6" t="s"/>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s"/>
     </row>
@@ -7761,16 +7763,14 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
+      <c r="B7" t="s"/>
       <c r="C7" t="s"/>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s"/>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -7781,11 +7781,11 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s"/>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s"/>
     </row>
@@ -7793,9 +7793,7 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
+      <c r="B9" t="s"/>
       <c r="C9" t="s"/>
       <c r="D9" t="s"/>
       <c r="E9" t="s"/>
@@ -7940,7 +7938,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s"/>
       <c r="D8" t="s"/>
@@ -8034,7 +8032,7 @@
       <c r="D2" t="s"/>
       <c r="E2" t="s"/>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -8080,7 +8078,7 @@
       </c>
       <c r="C6" t="s"/>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s"/>
       <c r="F6" t="s"/>
@@ -8092,7 +8090,7 @@
       <c r="B7" t="s"/>
       <c r="C7" t="s"/>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s"/>
       <c r="F7" t="s"/>
@@ -8242,7 +8240,9 @@
       <c r="B7" t="s"/>
       <c r="C7" t="s"/>
       <c r="D7" t="s"/>
-      <c r="E7" t="s"/>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
       <c r="F7" t="s"/>
     </row>
     <row r="8" spans="1:6">
@@ -8345,16 +8345,14 @@
         <v>21</v>
       </c>
       <c r="E2" t="s"/>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
+      <c r="F2" t="s"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -8365,7 +8363,9 @@
       <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s"/>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="n">
@@ -8375,11 +8375,9 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D4" t="s"/>
       <c r="E4" t="s"/>
       <c r="F4" t="s">
         <v>23</v>
@@ -8390,10 +8388,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -8411,28 +8409,30 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s"/>
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s"/>
-      <c r="F6" t="s"/>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s"/>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -8443,7 +8443,7 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s"/>
       <c r="E8" t="s"/>
@@ -8553,7 +8553,7 @@
       <c r="C3" t="s"/>
       <c r="D3" t="s"/>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s"/>
     </row>
@@ -8561,9 +8561,7 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
+      <c r="B4" t="s"/>
       <c r="C4" t="s"/>
       <c r="D4" t="s"/>
       <c r="E4" t="s"/>
@@ -8574,9 +8572,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s"/>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
+      <c r="C5" t="s"/>
       <c r="D5" t="s"/>
       <c r="E5" t="s"/>
       <c r="F5" t="s"/>
@@ -8587,11 +8583,11 @@
       </c>
       <c r="B6" t="s"/>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s"/>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s"/>
     </row>
@@ -8696,11 +8692,9 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s"/>
       <c r="D2" t="s">
         <v>9</v>
       </c>
@@ -8717,16 +8711,14 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s"/>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -8737,13 +8729,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -8760,10 +8752,10 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -8774,15 +8766,17 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s"/>
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
       <c r="F6" t="s">
         <v>16</v>
       </c>
@@ -8793,7 +8787,7 @@
       </c>
       <c r="B7" t="s"/>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -8814,11 +8808,11 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s"/>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -8826,9 +8820,11 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s"/>
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
@@ -8836,7 +8832,7 @@
         <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -8880,17 +8876,15 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s"/>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s"/>
+      <c r="F2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s"/>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -8901,13 +8895,13 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -8918,17 +8912,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s"/>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -8936,17 +8930,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="E5" t="s"/>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -8957,13 +8951,13 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -8980,7 +8974,9 @@
       <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s"/>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
       <c r="F7" t="s">
         <v>11</v>
       </c>
@@ -8996,9 +8992,11 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" t="s"/>
       <c r="F8" t="s">
         <v>10</v>
       </c>
@@ -9008,16 +9006,14 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
+      <c r="D9" t="s"/>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -9066,29 +9062,29 @@
       <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s"/>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
+      <c r="F2" t="s"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="s"/>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
       <c r="C3" t="s"/>
       <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E3" t="s"/>
       <c r="F3" t="s">
         <v>16</v>
       </c>
@@ -9098,10 +9094,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -9110,7 +9106,7 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -9118,16 +9114,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
@@ -9138,7 +9134,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -9150,7 +9146,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -9161,14 +9157,14 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s"/>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -9179,13 +9175,13 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s"/>
     </row>
@@ -9195,10 +9191,10 @@
       </c>
       <c r="B9" t="s"/>
       <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
         <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -9247,16 +9243,18 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="s"/>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s"/>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -9267,30 +9265,28 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F3" t="s"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -9304,10 +9300,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
       </c>
       <c r="D5" t="s"/>
       <c r="E5" t="s">
@@ -9322,17 +9318,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s"/>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
       <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
         <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -9340,7 +9338,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s"/>
       <c r="D7" t="s">
@@ -9356,10 +9354,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -9368,7 +9366,7 @@
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -9379,16 +9377,14 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
+      <c r="E9" t="s"/>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -9434,7 +9430,9 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s"/>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
@@ -9449,9 +9447,7 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
+      <c r="B3" t="s"/>
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -9470,13 +9466,11 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s"/>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s"/>
+      <c r="E4" t="s"/>
       <c r="F4" t="s">
         <v>8</v>
       </c>
@@ -9516,7 +9510,7 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -9527,7 +9521,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -9544,7 +9538,9 @@
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s"/>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>

</xml_diff>